<commit_message>
finished randomize balloons, still dependent of excel file
</commit_message>
<xml_diff>
--- a/trialTypes.xlsx
+++ b/trialTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="3">
   <si>
     <t xml:space="preserve">imageFile</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">blueBalloon.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redBalloon.png</t>
   </si>
 </sst>
 </file>
@@ -128,10 +125,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -158,30 +155,236 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
modify according to suggestions
</commit_message>
<xml_diff>
--- a/trialTypes.xlsx
+++ b/trialTypes.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="5">
   <si>
-    <t>imageFile</t>
+    <t>randomBalloon</t>
   </si>
   <si>
-    <t>maxPump</t>
+    <t>maxPumps</t>
   </si>
   <si>
-    <t>blue</t>
+    <t>redBalloon</t>
   </si>
   <si>
-    <t>red</t>
+    <t>greenBalloon</t>
   </si>
   <si>
-    <t>green</t>
+    <t>blueBalloon</t>
   </si>
 </sst>
 </file>
@@ -405,15 +405,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -429,15 +429,15 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -445,15 +445,15 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -461,79 +461,79 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -541,23 +541,23 @@
         <v>3</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -565,15 +565,15 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -581,23 +581,23 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -605,44 +605,44 @@
         <v>3</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -650,23 +650,23 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -674,15 +674,15 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -690,95 +690,95 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -786,47 +786,47 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B50">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B51">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B52">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B55">
         <v>7</v>
@@ -834,119 +834,119 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B59">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B60">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B62">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B63">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B64">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B65">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B67">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B70">
         <v>22</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71">
         <v>20</v>
@@ -962,162 +962,162 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B72">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B73">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B74">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B75">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B76">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B77">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B78">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B79">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B80">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B81">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B82">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B83">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B84">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B85">
-        <v>60</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B86">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B87">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B88">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B89">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B90">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B91">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added few words, add controls text
</commit_message>
<xml_diff>
--- a/trialTypes.xlsx
+++ b/trialTypes.xlsx
@@ -22,13 +22,13 @@
     <t>maxPumps</t>
   </si>
   <si>
-    <t>redBalloon</t>
+    <t>blueBalloon</t>
   </si>
   <si>
     <t>greenBalloon</t>
   </si>
   <si>
-    <t>blueBalloon</t>
+    <t>redBalloon</t>
   </si>
 </sst>
 </file>
@@ -405,47 +405,47 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -469,15 +469,15 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -485,84 +485,84 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -570,26 +570,26 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -597,15 +597,15 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -613,15 +613,15 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -629,68 +629,68 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -698,39 +698,39 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -746,58 +746,58 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -805,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B52">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -813,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B55">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -837,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B57">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -861,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -869,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="B60">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -885,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -893,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B63">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="B64">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="B65">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -917,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="B67">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -933,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -949,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="B70">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -957,164 +957,164 @@
         <v>3</v>
       </c>
       <c r="B71">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B72">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B73">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B74">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B75">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B76">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B78">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B79">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B80">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B81">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B82">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B83">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B84">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B85">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B86">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B87">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B88">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B89">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B90">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B91">
         <v>30</v>

</xml_diff>

<commit_message>
remove unused field in data file
</commit_message>
<xml_diff>
--- a/trialTypes.xlsx
+++ b/trialTypes.xlsx
@@ -405,15 +405,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -421,39 +421,39 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -466,50 +466,50 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -517,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -525,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -538,34 +538,34 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -573,23 +573,23 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -597,31 +597,31 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -629,15 +629,15 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -645,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -701,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -709,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -717,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -725,7 +725,7 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -749,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -757,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -781,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -797,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -805,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B52">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -813,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="B53">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B54">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B55">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -837,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B57">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="B58">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -861,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="B59">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -869,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="B60">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="B61">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -885,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B62">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -893,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B63">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="B64">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -909,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="B65">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -917,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="B66">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -925,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="B67">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -933,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="B68">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="B69">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -949,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="B70">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -957,7 +957,7 @@
         <v>3</v>
       </c>
       <c r="B71">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -973,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="B73">
-        <v>16</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -981,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="B74">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="B75">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="B76">
-        <v>11</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1005,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="B77">
-        <v>7</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1013,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="B78">
-        <v>11</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1021,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="B80">
-        <v>56</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1037,7 +1037,7 @@
         <v>2</v>
       </c>
       <c r="B81">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1045,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="B82">
-        <v>34</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1053,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="B83">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1061,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="B84">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1069,7 +1069,7 @@
         <v>2</v>
       </c>
       <c r="B85">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="B86">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="B87">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1093,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="B88">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1101,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="B89">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1109,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="B90">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1117,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="B91">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last bart test using python3
</commit_message>
<xml_diff>
--- a/trialTypes.xlsx
+++ b/trialTypes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>randomBalloon</t>
   </si>
@@ -22,10 +23,10 @@
     <t>maxPumps</t>
   </si>
   <si>
-    <t>blueBalloon</t>
+    <t>greenBalloon</t>
   </si>
   <si>
-    <t>greenBalloon</t>
+    <t>blueBalloon</t>
   </si>
   <si>
     <t>redBalloon</t>
@@ -35,26 +36,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,35 +66,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -385,12 +373,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
@@ -404,79 +398,79 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>122</v>
+      <c r="B2" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>52</v>
+      <c r="B3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>11</v>
+      <c r="B5" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>39</v>
+      <c r="B6" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>105</v>
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>104</v>
+        <v>4</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>67</v>
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
         <v>4</v>
       </c>
     </row>
@@ -484,167 +478,167 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12">
-        <v>5</v>
+      <c r="B12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>6</v>
+      <c r="B13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B14" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B15" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B16" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
-        <v>10</v>
+      <c r="B17" t="n">
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19">
-        <v>95</v>
+      <c r="B19" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20">
-        <v>115</v>
+        <v>4</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B21" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23">
-        <v>3</v>
+      <c r="B23" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>54</v>
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25">
-        <v>7</v>
+      <c r="B25" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26">
-        <v>8</v>
+      <c r="B26" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B27" t="n">
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28">
-        <v>23</v>
+      <c r="B28" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="B29" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>2</v>
       </c>
     </row>
@@ -652,63 +646,63 @@
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33">
-        <v>5</v>
+      <c r="B33" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34">
-        <v>2</v>
+      <c r="B34" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35">
-        <v>7</v>
+      <c r="B35" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36">
-        <v>7</v>
+      <c r="B36" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37">
-        <v>4</v>
+      <c r="B37" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38">
-        <v>2</v>
+      <c r="B38" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39">
-        <v>2</v>
+      <c r="B39" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -716,411 +710,411 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41">
-        <v>2</v>
+      <c r="B41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42">
-        <v>4</v>
+      <c r="B42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43">
-        <v>5</v>
+      <c r="B43" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44">
-        <v>4</v>
+      <c r="B44" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45">
-        <v>6</v>
+      <c r="B45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46">
-        <v>6</v>
+      <c r="B46" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47">
-        <v>7</v>
+      <c r="B47" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48">
-        <v>4</v>
+      <c r="B48" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49">
-        <v>7</v>
+      <c r="B49" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B50">
-        <v>4</v>
+      <c r="B50" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51">
-        <v>3</v>
+      <c r="B51" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="B52" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B54" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="B55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="B57" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="B58" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B59" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B60" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="B61" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="B62" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B63" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="B64" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="B65" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B66" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B67" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="B68" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B69" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B70" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B71" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B72" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="B73" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74">
-        <v>117</v>
+        <v>3</v>
+      </c>
+      <c r="B74" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75">
-        <v>116</v>
+        <v>3</v>
+      </c>
+      <c r="B75" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="B76" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77">
-        <v>105</v>
+        <v>3</v>
+      </c>
+      <c r="B77" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78">
-        <v>54</v>
+        <v>3</v>
+      </c>
+      <c r="B78" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="B79" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80">
-        <v>91</v>
+        <v>3</v>
+      </c>
+      <c r="B80" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81">
-        <v>79</v>
+        <v>3</v>
+      </c>
+      <c r="B81" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82">
-        <v>90</v>
+        <v>3</v>
+      </c>
+      <c r="B82" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="B83" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84">
-        <v>113</v>
+        <v>3</v>
+      </c>
+      <c r="B84" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85">
-        <v>98</v>
+        <v>3</v>
+      </c>
+      <c r="B85" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="B86" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="B87" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88">
-        <v>74</v>
+        <v>3</v>
+      </c>
+      <c r="B88" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89">
-        <v>102</v>
+        <v>3</v>
+      </c>
+      <c r="B89" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="B90" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91">
-        <v>49</v>
+        <v>3</v>
+      </c>
+      <c r="B91" t="n">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>